<commit_message>
chore: ajuste de identidade do app e inclusão das imagens do projeto
</commit_message>
<xml_diff>
--- a/Agregador_IR.xlsx
+++ b/Agregador_IR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humberto\Desktop\DIO\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\humberto\Desktop\DIO\Excel\excel-agregador-imposto-renda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCEBA77-CA07-486F-8001-A8DDE54C6066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EFAC99-8930-4324-AD31-0D28B4F927CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="0" xr2:uid="{21AF5686-43DE-436F-830C-EAB08FC5D1D8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>NOME</t>
   </si>
@@ -98,21 +98,6 @@
     <t>NÃO</t>
   </si>
   <si>
-    <t>FELIPE SKYWALKER NOBUNAGA</t>
-  </si>
-  <si>
-    <t>felipe@dio.me</t>
-  </si>
-  <si>
-    <t>Rua Dos limoeiros. R, - Nº 180</t>
-  </si>
-  <si>
-    <t>Rua Dos limoeiros. Ruan, - Nº 180</t>
-  </si>
-  <si>
-    <t>Mia Goth</t>
-  </si>
-  <si>
     <t>2. INFORMES DE RENDIMENTOS BANCÁRIOS</t>
   </si>
   <si>
@@ -315,6 +300,24 @@
   </si>
   <si>
     <t>HOLERITE</t>
+  </si>
+  <si>
+    <t>HUMBERTO ALCÂNTARA DE ARAPUJO JÚNIOR</t>
+  </si>
+  <si>
+    <t>CRIS ALCÂNTARA</t>
+  </si>
+  <si>
+    <t>AV. PORTUGAL</t>
+  </si>
+  <si>
+    <t>AV. PORTUGAL, 1290</t>
+  </si>
+  <si>
+    <t>humberto@</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
   </si>
 </sst>
 </file>
@@ -330,7 +333,7 @@
     <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="169" formatCode="mmmm\-yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,8 +442,23 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +491,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEE37BF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,7 +555,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -546,30 +570,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -589,6 +589,34 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
@@ -600,6 +628,10 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -786,7 +818,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
+      <xdr:colOff>1987550</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -836,7 +868,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="pt-BR" sz="2000" b="1">
+            <a:rPr lang="pt-BR" sz="1800" b="1">
               <a:gradFill flip="none" rotWithShape="1">
                 <a:gsLst>
                   <a:gs pos="1000">
@@ -857,7 +889,7 @@
               </a:gradFill>
               <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>LION APP</a:t>
+            <a:t>IR DATA HUB</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -873,7 +905,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
+      <xdr:colOff>1987550</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>160336</xdr:rowOff>
     </xdr:to>
@@ -891,8 +923,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="85725" y="1704974"/>
-          <a:ext cx="1930400" cy="373062"/>
+          <a:off x="82550" y="1733549"/>
+          <a:ext cx="1905000" cy="369887"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -957,13 +989,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>74613</xdr:rowOff>
+      <xdr:rowOff>69055</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>74613</xdr:rowOff>
+      <xdr:rowOff>69055</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -979,8 +1011,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="82550" y="2170113"/>
-          <a:ext cx="1936750" cy="400050"/>
+          <a:off x="82550" y="2221705"/>
+          <a:ext cx="1908175" cy="419100"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1033,8 +1065,8 @@
       <xdr:rowOff>187325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>192087</xdr:rowOff>
     </xdr:to>
@@ -1101,15 +1133,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>163512</xdr:rowOff>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1800226</xdr:colOff>
+      <xdr:colOff>1809750</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1587</xdr:rowOff>
+      <xdr:rowOff>87312</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1124,8 +1156,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="225425" y="3476625"/>
-          <a:ext cx="1574801" cy="447675"/>
+          <a:off x="349250" y="3659187"/>
+          <a:ext cx="1460500" cy="466725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1164,12 +1196,47 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>SYSTEM BY DIO </a:t>
+            <a:t>SMART EXCEL</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TAX SOLUTION </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:rPr lang="pt-BR" sz="1100" b="1" cap="none" spc="0">
+              <a:ln w="6600">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="accent2"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
             <a:t>💜</a:t>
           </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1234,15 +1301,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>882650</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>93662</xdr:rowOff>
+      <xdr:colOff>930275</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1227834</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>26988</xdr:rowOff>
+      <xdr:colOff>1275459</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>55563</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1273,8 +1340,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="885825" y="3810000"/>
-          <a:ext cx="345184" cy="333375"/>
+          <a:off x="930275" y="4141787"/>
+          <a:ext cx="345184" cy="333376"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1429,100 +1496,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Retângulo 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E4A9973-12D4-4891-A507-8F3029B54826}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="53975" y="104775"/>
-          <a:ext cx="1962150" cy="320675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="2000" b="1">
-              <a:gradFill flip="none" rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="1000">
-                    <a:schemeClr val="bg1"/>
-                  </a:gs>
-                  <a:gs pos="61000">
-                    <a:srgbClr val="EE37BF"/>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:srgbClr val="6124E8">
-                      <a:lumMod val="69000"/>
-                      <a:lumOff val="31000"/>
-                    </a:srgbClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="0" scaled="1"/>
-                <a:tileRect/>
-              </a:gradFill>
-              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>LION APP</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
+      <xdr:colOff>1987550</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -1594,8 +1574,8 @@
       <xdr:rowOff>55563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>36513</xdr:rowOff>
     </xdr:to>
@@ -1682,8 +1662,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
@@ -1750,83 +1730,6 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1800226</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628B5FFA-6B10-4B28-9335-4E2122034D41}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="225425" y="3473450"/>
-          <a:ext cx="1571626" cy="450850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="65000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SYSTEM BY DIO </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>💜</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
@@ -1878,68 +1781,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>882650</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1227834</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="icon_link" descr="Linkedin White Icons – Free Download SVG, PNG, GIF">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4206E5E7-4968-4CF8-A71C-26C4B64A84C0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="885825" y="3810000"/>
-          <a:ext cx="345184" cy="333375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
@@ -2072,6 +1913,267 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B4E674-97A4-4A4B-ACBB-1ABEFA09CCEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="104775"/>
+          <a:ext cx="1933575" cy="346075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="1000">
+                    <a:schemeClr val="bg1"/>
+                  </a:gs>
+                  <a:gs pos="61000">
+                    <a:srgbClr val="EE37BF"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="6124E8">
+                      <a:lumMod val="69000"/>
+                      <a:lumOff val="31000"/>
+                    </a:srgbClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="0" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>IR DATA HUB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1822450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Retângulo 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BDF7C81-13A3-45A2-A595-C6937D3B9286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361950" y="3648075"/>
+          <a:ext cx="1460500" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>SMART EXCEL</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TAX SOLUTION </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" cap="none" spc="0">
+              <a:ln w="6600">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="accent2"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>💜</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1288159</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>73026</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="icon_link" descr="Linkedin White Icons – Free Download SVG, PNG, GIF">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7753157A-6276-41CF-99CB-39A29F865D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="942975" y="4130675"/>
+          <a:ext cx="345184" cy="333376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2141,100 +2243,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Retângulo 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA3A21E-3032-4A44-9A60-D7C9B249346E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="53975" y="101600"/>
-          <a:ext cx="1962150" cy="327025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="2000" b="1">
-              <a:gradFill flip="none" rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="1000">
-                    <a:schemeClr val="bg1"/>
-                  </a:gs>
-                  <a:gs pos="61000">
-                    <a:srgbClr val="EE37BF"/>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:srgbClr val="6124E8">
-                      <a:lumMod val="69000"/>
-                      <a:lumOff val="31000"/>
-                    </a:srgbClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="0" scaled="1"/>
-                <a:tileRect/>
-              </a:gradFill>
-              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>LION APP</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2016125</xdr:colOff>
+      <xdr:colOff>1987550</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2306,8 +2321,8 @@
       <xdr:rowOff>87313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>68263</xdr:rowOff>
     </xdr:to>
@@ -2379,8 +2394,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2019300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2462,83 +2477,6 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1800226</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{992BA612-9853-4261-82C6-85FAB2FC725E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="225425" y="3476625"/>
-          <a:ext cx="1574801" cy="447675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="65000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>SYSTEM BY DIO </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>💜</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -2590,68 +2528,6 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>882650</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1227834</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="icon_link" descr="Linkedin White Icons – Free Download SVG, PNG, GIF">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFFA697F-D9BA-407E-A7E0-E9563EFB10B7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="885825" y="3810000"/>
-          <a:ext cx="345184" cy="333375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
@@ -2717,6 +2593,267 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61648AC1-70C7-4A28-B544-14DDE33DF3D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="104775"/>
+          <a:ext cx="1933575" cy="346075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1800" b="1">
+              <a:gradFill flip="none" rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="1000">
+                    <a:schemeClr val="bg1"/>
+                  </a:gs>
+                  <a:gs pos="61000">
+                    <a:srgbClr val="EE37BF"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:srgbClr val="6124E8">
+                      <a:lumMod val="69000"/>
+                      <a:lumOff val="31000"/>
+                    </a:srgbClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="0" scaled="1"/>
+                <a:tileRect/>
+              </a:gradFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>IR DATA HUB</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1841500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558F40F0-B2C8-4968-B4D8-3BD66330741C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="381000" y="3600450"/>
+          <a:ext cx="1460500" cy="466725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>SMART EXCEL</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TAX SOLUTION </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" cap="none" spc="0">
+              <a:ln w="6600">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="accent2"/>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>💜</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1307209</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>206376</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="icon_link" descr="Linkedin White Icons – Free Download SVG, PNG, GIF">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12B66617-3450-45C3-96A3-7476E18A6D35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="962025" y="4083050"/>
+          <a:ext cx="345184" cy="333376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2728,7 +2865,7 @@
     <tableColumn id="2" xr3:uid="{F34F7F55-794C-46B5-A546-FE1070EE20E7}" name="CATEGORIA" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{9B7F950C-CEE2-4840-870F-46DA94161C69}" name="VALOR" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
@@ -3053,7 +3190,7 @@
   <dimension ref="A3:E19"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,25 +3208,25 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>18</v>
+      <c r="D6" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="15">
         <v>12312312398</v>
       </c>
     </row>
@@ -3097,7 +3234,7 @@
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="16">
         <v>34605</v>
       </c>
     </row>
@@ -3105,7 +3242,7 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="14">
         <v>31713388</v>
       </c>
     </row>
@@ -3113,39 +3250,39 @@
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>22</v>
+      <c r="D10" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>21</v>
+      <c r="D11" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>20</v>
+      <c r="D12" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="12">
-        <v>987654321</v>
+      <c r="D13" s="17">
+        <v>55000000</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="18">
         <v>1131713388</v>
       </c>
     </row>
@@ -3153,7 +3290,7 @@
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="19">
         <v>11931713388</v>
       </c>
     </row>
@@ -3161,15 +3298,15 @@
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>19</v>
+      <c r="D16" s="20" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3177,7 +3314,7 @@
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="14" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3185,12 +3322,12 @@
       <c r="C19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="14" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:E4"/>
   </mergeCells>
@@ -3213,7 +3350,7 @@
   <dimension ref="A3:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,119 +3362,119 @@
   <sheetData>
     <row r="3" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="6" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <f>SUM(D11,D16,D21)</f>
-        <v>58377777</v>
-      </c>
-      <c r="D7" s="22"/>
+        <v>15391376</v>
+      </c>
+      <c r="D7" s="23"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="16">
-        <v>500000</v>
+        <v>21</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1000000</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="16">
-        <v>1312312</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="10">
+        <v>5845855</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="16">
-        <v>56565465</v>
+        <v>21</v>
+      </c>
+      <c r="D21" s="10">
+        <v>8545521</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:D7"/>
@@ -3365,7 +3502,7 @@
   <dimension ref="A3:E35"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,179 +3513,185 @@
   <sheetData>
     <row r="3" spans="3:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="3:5" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="7" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C7" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="17">
-        <v>45775</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="19">
-        <v>3000</v>
+      <c r="C9" s="11">
+        <v>45992</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="13">
+        <v>5600</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
+      <c r="C10" s="25">
+        <v>45992</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="13">
+        <v>9500</v>
+      </c>
     </row>
     <row r="11" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
     </row>
     <row r="32" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" spans="3:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C7:E7"/>
@@ -3579,257 +3722,257 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>